<commit_message>
Solo faltan pruebas de la primera col
</commit_message>
<xml_diff>
--- a/CVDS-LAB08/ClasesDeEquivalencia.xlsx
+++ b/CVDS-LAB08/ClasesDeEquivalencia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Desktop\CVDS\CVDS-LAB08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4138B7B8-EA72-4F03-AE07-3F22DA6CC12F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D601AE-15FF-477F-B784-6B3D43009CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17447" yWindow="193" windowWidth="12800" windowHeight="6000" xr2:uid="{8E649EE2-C05A-4574-AFF5-762806365EF1}"/>
+    <workbookView xWindow="19167" yWindow="933" windowWidth="12800" windowHeight="6000" xr2:uid="{8E649EE2-C05A-4574-AFF5-762806365EF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="71">
   <si>
     <t xml:space="preserve">Número </t>
   </si>
@@ -288,12 +288,6 @@
     <t>fechaDevolucion</t>
   </si>
   <si>
-    <t>fechaDevolucion &lt; fechaDeRenta</t>
-  </si>
-  <si>
-    <t>fechaDevolucion &gt;= fechaDeRenta</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Incorrecto/ </t>
     </r>
@@ -685,6 +679,43 @@
   </si>
   <si>
     <t xml:space="preserve">El  Item No existe en la base de datos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El item No existe </t>
+  </si>
+  <si>
+    <t>fechaDevolucion &lt;  fechaInicioDeRenta</t>
+  </si>
+  <si>
+    <t>fechaDevolucion &gt;= fechaInicioDeRenta  ∧  fechaDevolucion&gt; fechaFinEntrega</t>
+  </si>
+  <si>
+    <t>fechaFinEntrega &gt;= fechaDevolucion &gt;= fechaInicioDeRenta</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Correcto /</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1189,17 +1220,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49330D31-392B-4C26-9F4F-3331264FB7CD}">
-  <dimension ref="B1:R43"/>
+  <dimension ref="B1:R46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="3" max="3" width="23.3515625" customWidth="1"/>
     <col min="4" max="4" width="34.41015625" customWidth="1"/>
-    <col min="9" max="9" width="26.234375" customWidth="1"/>
+    <col min="9" max="9" width="47.41015625" customWidth="1"/>
     <col min="10" max="10" width="46.3515625" customWidth="1"/>
     <col min="11" max="11" width="26.87890625" customWidth="1"/>
     <col min="15" max="15" width="14" customWidth="1"/>
@@ -1221,7 +1252,7 @@
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="M1" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N1" s="10"/>
       <c r="O1" s="10"/>
@@ -1278,16 +1309,16 @@
       <c r="J3" s="6"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="R3" s="2"/>
     </row>
@@ -1296,7 +1327,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>5</v>
@@ -1305,31 +1336,31 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M4" s="2">
         <v>1</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="43" x14ac:dyDescent="0.5">
@@ -1337,7 +1368,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>4</v>
@@ -1346,28 +1377,28 @@
         <v>2</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>22</v>
+        <v>69</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="M5" s="2">
         <v>2</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>12</v>
@@ -1381,28 +1412,28 @@
         <v>3</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="M6" s="2">
         <v>3</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>4</v>
@@ -1412,514 +1443,553 @@
       <c r="B7" s="1"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
+      <c r="G7" s="3">
+        <v>4</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="M7" s="2">
         <v>4</v>
       </c>
       <c r="N7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="43" x14ac:dyDescent="0.5">
+      <c r="B8" s="1"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="G8" s="3">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.5">
+      <c r="B9" s="1"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.5">
+      <c r="B10" s="1"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.5">
+      <c r="B11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.5">
+      <c r="B12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="12"/>
+      <c r="J12" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.5">
+      <c r="B13" s="6"/>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="2:18" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="G16" s="3">
+        <v>3</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="G17" s="1"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="B18" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="G18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="B19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="12"/>
+      <c r="J19" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="B20" s="6"/>
+      <c r="C20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="2:10" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="B22" s="3">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="3">
+        <v>2</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="B23" s="3">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="3">
+        <v>3</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="B25" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="G25" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="B26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="12"/>
+      <c r="J26" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="B27" s="6"/>
+      <c r="C27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="2:10" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="71.7" x14ac:dyDescent="0.5">
+      <c r="B29" s="3">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="3">
+        <v>2</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="B30" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="B31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="B32" s="6"/>
+      <c r="C32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="2:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="B34" s="3">
+        <v>2</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.5">
+      <c r="B36" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.5">
+      <c r="B37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.5">
+      <c r="B38" s="6"/>
+      <c r="C38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="2:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="B40" s="3">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.5">
-      <c r="B8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="G8" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.5">
-      <c r="B9" s="4" t="s">
+      <c r="F40" s="2"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.5">
+      <c r="B42" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.5">
+      <c r="B43" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.5">
-      <c r="B10" s="6"/>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="2:18" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="3">
-        <v>1</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="B12" s="3">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="3">
-        <v>2</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="G13" s="3">
-        <v>3</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.5">
-      <c r="G14" s="1"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.5">
-      <c r="B15" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="G15" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.5">
-      <c r="B16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.5">
-      <c r="B17" s="6"/>
-      <c r="C17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="2:10" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="3">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="B19" s="3">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="3">
-        <v>2</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="B20" s="3">
-        <v>3</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="3">
-        <v>3</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I20" s="2" t="s">
+      <c r="C43" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.5">
+      <c r="B44" s="6"/>
+      <c r="C44" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="2:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="B45" s="3">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.5">
-      <c r="B22" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="G22" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.5">
-      <c r="B23" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I23" s="12"/>
-      <c r="J23" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.5">
-      <c r="B24" s="6"/>
-      <c r="C24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J24" s="6"/>
-    </row>
-    <row r="25" spans="2:10" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" s="3">
-        <v>1</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" ht="71.7" x14ac:dyDescent="0.5">
-      <c r="B26" s="3">
-        <v>2</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26" s="3">
-        <v>2</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.5">
-      <c r="B27" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.5">
-      <c r="B28" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.5">
-      <c r="B29" s="6"/>
-      <c r="C29" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="2:10" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="B30" s="3">
-        <v>1</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="B31" s="3">
-        <v>2</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.5">
-      <c r="B33" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.5">
-      <c r="B34" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.5">
-      <c r="B35" s="6"/>
-      <c r="C35" s="2" t="s">
+    </row>
+    <row r="46" spans="2:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="B46" s="3">
+        <v>2</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="2:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="B36" s="3">
-        <v>1</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="B37" s="3">
-        <v>2</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.5">
-      <c r="B39" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.5">
-      <c r="B40" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.5">
-      <c r="B41" s="6"/>
-      <c r="C41" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D41" s="7"/>
-    </row>
-    <row r="42" spans="2:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="B42" s="3">
-        <v>1</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="B43" s="3">
-        <v>2</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>48</v>
+      <c r="D46" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="M1:R1"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B18:D18"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="G1:J1"/>
-    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B25:D25"/>
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>